<commit_message>
Websites of the components are added
</commit_message>
<xml_diff>
--- a/Component Selection/Component List.xlsx
+++ b/Component Selection/Component List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\masaüstü\4.sınıf\1.dönem\EE463-Static Power Conversion 1\Term Project\Project\Component Selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DD653E-92A3-4E02-9107-A645A14B502E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73F19EF-EFA4-464C-8D17-1567721E3392}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
   <si>
     <t>Component</t>
   </si>
@@ -233,6 +233,18 @@
   </si>
   <si>
     <t>240V (max), 210V(Rated);  5A (max), 2A (Rated)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/united-chemi-con/EKXJ221ELL101MK25S/3528962</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/CC0100KRX5R4BB102/11490370</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/illinois-capacitor/107RZM050M/5410782?s=N4IgTCBcDaIIwAYDsAlAWgWQQVhAXQF8g</t>
   </si>
 </sst>
 </file>
@@ -298,7 +310,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -442,87 +454,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -533,9 +469,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -545,32 +479,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -580,63 +505,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -917,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H42"/>
+  <dimension ref="B1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -932,522 +850,561 @@
     <col min="6" max="6" width="19.5546875" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
     <col min="8" max="8" width="10.21875" customWidth="1"/>
+    <col min="9" max="9" width="117" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="6" t="s">
+      <c r="I2" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>0.25</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="7"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="6"/>
-      <c r="C4" s="2" t="s">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="27"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="20"/>
+      <c r="C4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="6"/>
-      <c r="C5" s="12" t="s">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="27"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="20"/>
+      <c r="C5" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="6"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="6"/>
-      <c r="C7" s="2" t="s">
+      <c r="D5" s="19"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="27"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="20"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="27"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="20"/>
+      <c r="C7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="6"/>
-      <c r="C8" s="2">
+      <c r="D7" s="19"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="27"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="20"/>
+      <c r="C8" s="1">
         <v>560</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="6"/>
-      <c r="C9" s="2" t="s">
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="27"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="20"/>
+      <c r="C9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="6"/>
-      <c r="C10" s="12" t="s">
+      <c r="D9" s="19"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="27"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="20"/>
+      <c r="C10" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="6"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="6"/>
-      <c r="C12" s="2">
+      <c r="D10" s="19"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="27"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="20"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="27"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="20"/>
+      <c r="C12" s="1">
         <v>240</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="6"/>
-      <c r="C13" s="2" t="s">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="27"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="20"/>
+      <c r="C13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="6"/>
-      <c r="C14" s="2" t="s">
+      <c r="D13" s="19"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="27"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="20"/>
+      <c r="C14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="6"/>
-      <c r="C15" s="2" t="s">
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="27"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="20"/>
+      <c r="C15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="6"/>
-      <c r="C16" s="12" t="s">
+      <c r="D15" s="19"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="27"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="20"/>
+      <c r="C16" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="6"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="6"/>
-      <c r="C18" s="2">
+      <c r="D16" s="19"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="27"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="20"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="27"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="20"/>
+      <c r="C18" s="1">
         <v>680</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="6"/>
-      <c r="C19" s="12">
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="27"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="20"/>
+      <c r="C19" s="19">
         <v>820</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="6"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="6"/>
-      <c r="C21" s="12" t="s">
+      <c r="D19" s="19"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="27"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="20"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="27"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="20"/>
+      <c r="C21" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="6"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="6"/>
-      <c r="C23" s="2" t="s">
+      <c r="D21" s="19"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="27"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="20"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="27"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="20"/>
+      <c r="C23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="6"/>
-      <c r="C24" s="2" t="s">
+      <c r="D23" s="19"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="27"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B24" s="20"/>
+      <c r="C24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="6"/>
-      <c r="C25" s="2" t="s">
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="27"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B25" s="20"/>
+      <c r="C25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="6"/>
-      <c r="C26" s="2" t="s">
+      <c r="D25" s="19"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="27"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B26" s="20"/>
+      <c r="C26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="7"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="6" t="s">
+      <c r="D26" s="19"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="27"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B27" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F27" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G27" s="26" t="s">
+      <c r="G27" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27" s="1">
         <v>2.8559999999999999E-2</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="6"/>
-      <c r="C28" s="2" t="s">
+      <c r="I27" s="27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B28" s="20"/>
+      <c r="C28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G28" s="26" t="s">
+      <c r="G28" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="1">
         <v>0.71257999999999999</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="6"/>
-      <c r="C29" s="2" t="s">
+      <c r="I28" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B29" s="20"/>
+      <c r="C29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G29" s="26" t="s">
+      <c r="G29" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H29" s="1">
         <v>1.4749999999999999E-2</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="8" t="s">
+      <c r="I29" s="27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B30" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="7"/>
-    </row>
-    <row r="31" spans="2:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B31" s="8" t="s">
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="27"/>
+    </row>
+    <row r="31" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B31" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="7"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="6" t="s">
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="27"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B32" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1" t="s">
+      <c r="C32" s="19"/>
+      <c r="D32" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="16"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="6"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="17"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="6"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="17"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="6"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="17"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="6"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="17"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B37" s="6"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="18"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="6"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2" t="s">
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="27"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B33" s="20"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="27"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B34" s="20"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="27"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B35" s="20"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="27"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B36" s="20"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="27"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B37" s="20"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="27"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B38" s="20"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="7"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B39" s="6"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2" t="s">
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="27"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B39" s="20"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="7"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="6"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2" t="s">
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="27"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B40" s="20"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="7"/>
-    </row>
-    <row r="41" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="9" t="s">
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="27"/>
+    </row>
+    <row r="41" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10" t="s">
+      <c r="C41" s="7"/>
+      <c r="D41" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="11"/>
-    </row>
-    <row r="42" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G42" s="31" t="s">
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="28"/>
+    </row>
+    <row r="42" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G42" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="H42" s="32">
+      <c r="H42" s="24">
         <f>SUM(H3:H41)</f>
         <v>0.75589000000000006</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D18:D23"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E32:E37"/>
-    <mergeCell ref="F32:F37"/>
-    <mergeCell ref="G32:G37"/>
     <mergeCell ref="H32:H37"/>
     <mergeCell ref="B3:B26"/>
     <mergeCell ref="B27:B29"/>
@@ -1458,6 +1415,16 @@
     <mergeCell ref="D8:D11"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="D14:D17"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E32:E37"/>
+    <mergeCell ref="F32:F37"/>
+    <mergeCell ref="G32:G37"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C21:C22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G28" r:id="rId1" display="https://www.digikey.com/en/products/detail/united-chemi-con/EKXJ221ELL101MK25S/3528962" xr:uid="{85104F1A-C2B0-4CB9-A7C9-C5C7B81B29BC}"/>
@@ -1486,90 +1453,90 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="19"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>0.32</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B4" s="22"/>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="21"/>
+      <c r="C4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="13">
         <v>2.8559999999999999E-2</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="23"/>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="7">
         <v>5.6070000000000002E-2</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="19"/>
-      <c r="C7" s="20" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>0.79042999999999997</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="23"/>
-      <c r="C9" s="24" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="17">
         <v>0.71257999999999999</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="18" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="28"/>
+      <c r="B10" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>